<commit_message>
Add Excell zu Binomial
</commit_message>
<xml_diff>
--- a/Binomial_Pascal.xlsx
+++ b/Binomial_Pascal.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neveling.net\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -105,6 +105,38 @@
     </r>
     <r>
       <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -120,7 +152,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Das Diagramm zeigt den Aufwand bei zunehmender Pascalreihe. </t>
+      <t xml:space="preserve"> Das Diagramm zeigt den Aufwand bei zunehmender Pascalreihe. Die Skalierung ist bei beiden AchsenLogarithmisch.</t>
     </r>
   </si>
 </sst>
@@ -128,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +181,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -274,8 +314,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1234838145231846"/>
-          <c:y val="0.12962962962962962"/>
+          <c:x val="0.12348373331050315"/>
+          <c:y val="0.11443509732223643"/>
           <c:w val="0.81862729658792655"/>
           <c:h val="0.74350320793234181"/>
         </c:manualLayout>
@@ -1288,15 +1328,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>628649</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1495425</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1621,19 +1661,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="42.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
     <col min="12" max="12" width="20.28515625" customWidth="1"/>
     <col min="13" max="13" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1641,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1649,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1657,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1665,7 +1708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1673,21 +1716,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="L6" t="s">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1695,7 +1732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1703,21 +1740,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
-      <c r="L9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1725,7 +1756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20</v>
       </c>
@@ -1733,7 +1764,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>30</v>
       </c>
@@ -1741,7 +1772,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>40</v>
       </c>
@@ -1749,7 +1780,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
@@ -1757,7 +1788,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>60</v>
       </c>
@@ -1765,15 +1796,21 @@
         <v>465</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
       <c r="B16">
         <v>630</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>80</v>
       </c>
@@ -1781,7 +1818,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>90</v>
       </c>
@@ -1789,12 +1826,20 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>100</v>
       </c>
       <c r="B19">
         <v>1275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>